<commit_message>
1. Improve monthly hour report excel
</commit_message>
<xml_diff>
--- a/report_template/dailyReport.xlsx
+++ b/report_template/dailyReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\webApp\Datalogger2\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\Datalogger2\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D82515D-5C4F-4DBD-8D4F-95F8A35B872D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFE10F3-9D3C-43F9-9C00-F806EDDC185C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="6300" windowWidth="23580" windowHeight="17010" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
+    <workbookView xWindow="2400" yWindow="1005" windowWidth="25590" windowHeight="13365" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -187,28 +187,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -529,25 +529,25 @@
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -557,153 +557,153 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>0.375</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>0.625</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>0.875</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>